<commit_message>
atualização e testes de integração
</commit_message>
<xml_diff>
--- a/docs/Engenharia de Software/BEC_EngSW_Requisitos.xlsx
+++ b/docs/Engenharia de Software/BEC_EngSW_Requisitos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16ED9627-62F3-4D13-B94E-15056EFEB3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01897409-781D-45C5-B962-174BE45CB408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RequisitosFuncionais" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -136,36 +139,18 @@
     <t>O sistema deve conter uma caixa de diálogo com texto válido de (1 - 3000) caracteres, processar o texto e convertê-lo para imagem png.</t>
   </si>
   <si>
-    <t>O sistema deve suportar jpeg. png. jpg. A IA deve converter a imagem enviada em um modelo 3D obj. ou stl.</t>
-  </si>
-  <si>
-    <t>O sistema deve suportar upload de arquivos obj. stl. fatiar e gerar o arquivo G-code a partir de um modelo 3D</t>
-  </si>
-  <si>
     <t>O sistema deve emitir notas fiscais eletrônicas de forma automática após o pagamento do pedido ser efetuado</t>
   </si>
   <si>
     <t>O sistema deve realizar a geração de orçamentos dos arquivos de g-code no carrinho do cliente</t>
   </si>
   <si>
-    <t>O sistema deve manter um histórico de pedidos, conversões e transações da conta.</t>
-  </si>
-  <si>
     <t>Onde que vai ficar e para quem vai aparecer o historico</t>
   </si>
   <si>
-    <t>O sistema deve oferecer integração com métodos de pagamento, boleto</t>
-  </si>
-  <si>
     <t>Correção de ortografia</t>
   </si>
   <si>
-    <t>O sistema deve permitir adição, remoção dos itens do pedido. Deve ter uma página dedicada para exibir os itens selecionados.</t>
-  </si>
-  <si>
-    <t>O sistema deve permitir criação e cancelamento da ordem de compra</t>
-  </si>
-  <si>
     <t>O sistema deve permitir o acompanhamento do status (Pagamento Efetuado, Imprimindo, Impressão finalizada, Enviado, Entregue) de cada pedido</t>
   </si>
   <si>
@@ -197,6 +182,36 @@
   </si>
   <si>
     <t>NF-006</t>
+  </si>
+  <si>
+    <t>O sistema deve suportar jpeg. png. jpg. A IA deve converter a imagem enviada pelo cliente em um modelo 3D obj. ou stl.</t>
+  </si>
+  <si>
+    <t>O sistema deve manter um histórico de pedidos, conversões e transações da conta do cliente.</t>
+  </si>
+  <si>
+    <t>O sistema deve oferecer integração com  o método de pagamento, boleto. E oferecer como método de pagamento para finalizar a compra</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir adição, remoção dos itens do pedido do cliente. Deve ter uma página dedicada para exibir os itens selecionados.</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir criação e cancelamento da ordem de compra pelo cliente</t>
+  </si>
+  <si>
+    <t>RF-012</t>
+  </si>
+  <si>
+    <t>RF-020</t>
+  </si>
+  <si>
+    <t>O sistema deve suportar upload de arquivos obj. stl. Feito pelo cliente, fatiar e gerar o arquivo G-code a partir de um modelo 3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O Sistema deverá enviar o arquivo 3D ao finalizar o pedido do cliente para a impressora e iniciar a impressão. </t>
+  </si>
+  <si>
+    <t>O Sistema deve ajustar a impressora</t>
   </si>
 </sst>
 </file>
@@ -274,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -320,9 +335,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -610,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,14 +721,14 @@
       <c r="F5" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="15" t="s">
@@ -728,12 +740,12 @@
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="15" t="s">
@@ -750,7 +762,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="15" t="s">
@@ -767,7 +779,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="15" t="s">
@@ -784,7 +796,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="15" t="s">
@@ -795,15 +807,15 @@
         <v>35</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>44</v>
+      <c r="B11" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="15" t="s">
@@ -814,7 +826,7 @@
         <v>36</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -822,7 +834,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="15" t="s">
@@ -833,7 +845,7 @@
         <v>35</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -841,7 +853,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="15" t="s">
@@ -852,7 +864,7 @@
         <v>35</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -860,7 +872,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="15" t="s">
@@ -873,11 +885,11 @@
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>49</v>
+      <c r="B15" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="15" t="s">
@@ -891,10 +903,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="14" t="s">
@@ -907,11 +919,11 @@
       <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>53</v>
+      <c r="A17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="14" t="s">
@@ -925,10 +937,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="14" t="s">
@@ -942,10 +954,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="14" t="s">
@@ -959,10 +971,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="14" t="s">
@@ -976,10 +988,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="14" t="s">
@@ -992,8 +1004,12 @@
       <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="6"/>
@@ -1001,8 +1017,12 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="6"/>
@@ -1010,7 +1030,9 @@
       <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1019,8 +1041,6 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="6"/>
@@ -1028,8 +1048,6 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="6"/>
@@ -1037,8 +1055,6 @@
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="6"/>
@@ -1046,8 +1062,6 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="6"/>
@@ -1055,8 +1069,6 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="6"/>
@@ -1064,8 +1076,6 @@
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="6"/>
@@ -1073,8 +1083,6 @@
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="6"/>

</xml_diff>